<commit_message>
Finish creating Division Dashboard and add it to DashboardBuilder.py function
</commit_message>
<xml_diff>
--- a/Data Files/conferences.xlsx
+++ b/Data Files/conferences.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rspoonmore/Documents/Coding/CollegeFootballBowlGames/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rspoonmore/Documents/Coding/CollegeFootballBowlGames/Data Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF954AAA-3877-C149-961D-5E0ACAD84284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6E408E-23F1-5149-BA25-7EB094ECFA43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9580" yWindow="2880" windowWidth="27640" windowHeight="16940" xr2:uid="{3263E9AF-F9C0-DC44-AEF2-F5BCA61BF551}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Old!$A$1:$F$288</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$391</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$390</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1184,7 +1184,7 @@
   <dimension ref="A1:F390"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1751,7 +1751,7 @@
         <v>243</v>
       </c>
       <c r="E28" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
       <c r="F28" t="s">
         <v>247</v>
@@ -2571,7 +2571,7 @@
         <v>243</v>
       </c>
       <c r="E69" t="s">
-        <v>243</v>
+        <v>255</v>
       </c>
       <c r="F69" t="s">
         <v>247</v>
@@ -4331,7 +4331,7 @@
         <v>243</v>
       </c>
       <c r="E157" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
       <c r="F157" t="s">
         <v>247</v>
@@ -5171,7 +5171,7 @@
         <v>243</v>
       </c>
       <c r="E199" t="s">
-        <v>243</v>
+        <v>255</v>
       </c>
       <c r="F199" t="s">
         <v>247</v>

</xml_diff>